<commit_message>
atualizei a minha parte do slide
</commit_message>
<xml_diff>
--- a/Documentação/Planejamentos/plano_de_acao.xlsx
+++ b/Documentação/Planejamentos/plano_de_acao.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>PLANO DE AÇÃO - CHAMALEON PROJECT</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Alta</t>
-  </si>
-  <si>
-    <t>Em processo</t>
   </si>
   <si>
     <t>27.04.2020</t>
@@ -921,7 +918,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -966,7 +963,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -977,272 +974,272 @@
         <v>8</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E6" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="11">
         <v>1</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="F9" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E11" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="11">
         <v>1</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="11">
         <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>10</v>
-      </c>
       <c r="E14" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>